<commit_message>
Jenkins için pom.xml e build eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaProjeler\Cucumber_Kursu2\src\test\java\ApachePOI\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu3\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8976" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Lion</t>
   </si>
@@ -63,62 +63,58 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulkeleris11</t>
-  </si>
-  <si>
-    <t>ulkeleris22</t>
-  </si>
-  <si>
-    <t>ulkeleris33</t>
-  </si>
-  <si>
-    <t>ulkeleris44</t>
-  </si>
-  <si>
-    <t>ulkeleris55</t>
-  </si>
-  <si>
-    <t>ulkeleris66</t>
-  </si>
-  <si>
-    <t>ulkeleris77</t>
-  </si>
-  <si>
-    <t>ulkeleris88</t>
-  </si>
-  <si>
-    <t>umis1</t>
-  </si>
-  <si>
-    <t>umis2</t>
-  </si>
-  <si>
-    <t>umis3</t>
-  </si>
-  <si>
-    <t>umis4</t>
-  </si>
-  <si>
-    <t>umis5</t>
-  </si>
-  <si>
-    <t>umis6</t>
-  </si>
-  <si>
-    <t>umis7</t>
-  </si>
-  <si>
-    <t>umis8</t>
-  </si>
-  <si>
-    <t>Merhaba Dünya</t>
+    <t>ulkemis11</t>
+  </si>
+  <si>
+    <t>ulkemis22</t>
+  </si>
+  <si>
+    <t>ulkemis33</t>
+  </si>
+  <si>
+    <t>ulkemis44</t>
+  </si>
+  <si>
+    <t>ulkemis55</t>
+  </si>
+  <si>
+    <t>ulkemis66</t>
+  </si>
+  <si>
+    <t>ulkemis77</t>
+  </si>
+  <si>
+    <t>ulkemis88</t>
+  </si>
+  <si>
+    <t>uis11</t>
+  </si>
+  <si>
+    <t>uis21</t>
+  </si>
+  <si>
+    <t>uis31</t>
+  </si>
+  <si>
+    <t>uis41</t>
+  </si>
+  <si>
+    <t>uis51</t>
+  </si>
+  <si>
+    <t>uis61</t>
+  </si>
+  <si>
+    <t>uis71</t>
+  </si>
+  <si>
+    <t>uis81</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,47 +427,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C1" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D1" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E1" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F1" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G1" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="H1" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I1" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="J1" t="n">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -485,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -493,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -501,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -509,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -517,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -525,7 +497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -541,15 +513,15 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.21875" collapsed="false"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -569,7 +541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -589,7 +561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -609,7 +581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -629,7 +601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -649,7 +621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -669,7 +641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -689,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>

</xml_diff>